<commit_message>
generate and save enrichment results to output files
</commit_message>
<xml_diff>
--- a/results/Module_go_enrichment_results.xlsx
+++ b/results/Module_go_enrichment_results.xlsx
@@ -876,7 +876,7 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -887,9 +887,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="43.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
@@ -6053,11 +6053,11 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.84"/>
@@ -8019,12 +8019,22 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>